<commit_message>
supp def cardiaque 2019 rsa
</commit_message>
<xml_diff>
--- a/formats/excel/Formats RSA 19.xlsx
+++ b/formats/excel/Formats RSA 19.xlsx
@@ -465,6 +465,12 @@
     <t xml:space="preserve">Numéro d'innovation</t>
   </si>
   <si>
+    <t xml:space="preserve">SUPPDEFCARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplément défibrillateur cardiaque</t>
+  </si>
+  <si>
     <t xml:space="preserve">CONVERSION_HC</t>
   </si>
   <si>
@@ -487,12 +493,6 @@
   </si>
   <si>
     <t xml:space="preserve">Séjour éligible au forfait diabète</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUPPDEFCARD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supplément défibrillateur cardiaque</t>
   </si>
   <si>
     <t xml:space="preserve">FILLER2</t>
@@ -569,6 +569,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -618,11 +619,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -645,8 +646,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D85" activeCellId="0" sqref="D85"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D78" activeCellId="0" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2201,10 +2202,10 @@
         <f aca="false">A74+C74-A75</f>
         <v>0</v>
       </c>
-      <c r="E74" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F74" s="1" t="s">
+      <c r="E74" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F74" s="2" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2222,10 +2223,10 @@
         <f aca="false">A75+C75-A76</f>
         <v>0</v>
       </c>
-      <c r="E75" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F75" s="1" t="s">
+      <c r="E75" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F75" s="2" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2243,10 +2244,10 @@
         <f aca="false">A76+C76-A77</f>
         <v>0</v>
       </c>
-      <c r="E76" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F76" s="1" t="s">
+      <c r="E76" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F76" s="2" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2264,28 +2265,28 @@
         <f aca="false">A77+C77-A78</f>
         <v>0</v>
       </c>
-      <c r="E77" s="0" t="s">
+      <c r="E77" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="78" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="2" t="n">
+    <row r="78" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="n">
         <v>197</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C78" s="2" t="n">
-        <v>8</v>
+      <c r="C78" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D78" s="0" t="n">
         <f aca="false">A78+C78-A79</f>
-        <v>4</v>
-      </c>
-      <c r="E78" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>